<commit_message>
TestNg.xml smoke test jenkins
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="16">
   <si>
     <t>Create and Delete CitizenShip from Excel</t>
   </si>
@@ -36,6 +36,30 @@
   </si>
   <si>
     <t>Login with valid username and password</t>
+  </si>
+  <si>
+    <t>States testing with JDBC</t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
+  </si>
+  <si>
+    <t>Create country</t>
+  </si>
+  <si>
+    <t>Create a country 2</t>
+  </si>
+  <si>
+    <t>Users List</t>
+  </si>
+  <si>
+    <t>Create New Exam</t>
+  </si>
+  <si>
+    <t>Create Nationality</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -80,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -295,6 +319,664 @@
         <v>2</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>